<commit_message>
Added Suggestions by Amandeep
</commit_message>
<xml_diff>
--- a/AadiGranthSahibTatkra.xlsx
+++ b/AadiGranthSahibTatkra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AadiGranth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C9EBD8-8BDA-4486-9275-C86C037DCEAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6D95BD-A5B4-4AC0-A15F-C416E8EFF312}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{B14D38C9-60DE-403E-BFFD-A4806722A9C1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="586">
   <si>
     <t>Baani</t>
   </si>
@@ -1780,6 +1780,15 @@
   </si>
   <si>
     <t>1429_1429_Mundavni_M5</t>
+  </si>
+  <si>
+    <t>AudioFormat</t>
+  </si>
+  <si>
+    <t>Viakhea by (Gurjeet Singh)</t>
+  </si>
+  <si>
+    <t>Viakhea in (Class)</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1805,7 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1804,25 +1813,19 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1917,24 +1920,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2249,45 +2254,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F307B0-605D-44FF-A022-FC6A3833764D}">
-  <dimension ref="A1:E582"/>
+  <dimension ref="A1:I582"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.06640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" customWidth="1"/>
+    <col min="7" max="7" width="22.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="4" t="s">
+    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2295,52 +2313,52 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>16</v>
       </c>

</xml_diff>